<commit_message>
Inclusão de algumas colunas na planilha; verificação de existência e inserção de Escolas e Alunos; pendente inserção dos títulos
</commit_message>
<xml_diff>
--- a/public/sample_titulos.xlsx
+++ b/public/sample_titulos.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BB_DENTAL" localSheetId="0">Plan1!$A$1:$L$6</definedName>
+    <definedName name="BB_DENTAL" localSheetId="0">Plan1!$A$1:$O$6</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>NOME</t>
   </si>
@@ -99,22 +99,37 @@
     <t>RENATO GOMES</t>
   </si>
   <si>
-    <t>SAO FRANCISCO</t>
-  </si>
-  <si>
     <t>RENATO</t>
   </si>
   <si>
     <t>ANA LUIZA</t>
   </si>
   <si>
-    <t>SAO JOSE</t>
-  </si>
-  <si>
     <t>ANA</t>
   </si>
   <si>
     <t>5514981225509</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>CIDADE</t>
+  </si>
+  <si>
+    <t>SÃO PAULO</t>
+  </si>
+  <si>
+    <t>SÃO FRANCISCO</t>
+  </si>
+  <si>
+    <t>SÃO JOSÉ</t>
+  </si>
+  <si>
+    <t>BAURU</t>
   </si>
 </sst>
 </file>
@@ -175,7 +190,64 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -191,19 +263,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -269,9 +338,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Plan1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="firstRowStripe" dxfId="16"/>
-      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -286,10 +355,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:L6" headerRowDxfId="4" dataDxfId="2" totalsRowDxfId="3">
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:O6" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15">
+  <tableColumns count="15">
     <tableColumn id="1" name="NOME" dataDxfId="14"/>
+    <tableColumn id="13" name="RG" dataDxfId="2"/>
     <tableColumn id="2" name="ESCOLA" dataDxfId="13"/>
+    <tableColumn id="15" name="ESTADO" dataDxfId="0"/>
+    <tableColumn id="14" name="CIDADE" dataDxfId="1"/>
     <tableColumn id="3" name="TURMA" dataDxfId="12"/>
     <tableColumn id="4" name="PERIODO" dataDxfId="11"/>
     <tableColumn id="5" name="TITULO" dataDxfId="10"/>
@@ -297,9 +369,9 @@
     <tableColumn id="7" name="CELULAR" dataDxfId="8"/>
     <tableColumn id="8" name="TELEFONE" dataDxfId="7"/>
     <tableColumn id="9" name="TELEFONE2" dataDxfId="6"/>
-    <tableColumn id="10" name="CELULAR2" dataDxfId="1"/>
-    <tableColumn id="11" name="VALOR" dataDxfId="0"/>
-    <tableColumn id="12" name="VENCIMENTO" dataDxfId="5"/>
+    <tableColumn id="10" name="CELULAR2" dataDxfId="5"/>
+    <tableColumn id="11" name="VALOR" dataDxfId="4"/>
+    <tableColumn id="12" name="VENCIMENTO" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Plan1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -602,231 +674,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="12.5703125" style="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="20" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="12.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>487562847</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1">
+      <c r="H2" s="1">
         <v>111</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="J2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1">
         <v>1432523294</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="M2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="5">
         <v>100</v>
       </c>
-      <c r="L2" s="4">
+      <c r="O2" s="4">
         <v>42900</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>444444444</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1">
+      <c r="H3" s="1">
         <v>222</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="J3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1">
         <v>1432523294</v>
       </c>
-      <c r="K3" s="5">
+      <c r="N3" s="5">
         <v>150</v>
       </c>
-      <c r="L3" s="4">
+      <c r="O3" s="4">
         <v>42901</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>555555555</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1">
+      <c r="H4" s="1">
         <v>333</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="J4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1">
         <v>1432523294</v>
       </c>
-      <c r="I4" s="1">
+      <c r="L4" s="1">
         <v>1432523294</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="5">
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="5">
         <v>150.56</v>
       </c>
-      <c r="L4" s="4">
+      <c r="O4" s="4">
         <v>42902</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="1">
+        <v>666666666</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1">
+        <v>444</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1">
-        <v>444</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="J5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1432523294</v>
+      </c>
+      <c r="N5" s="5">
+        <v>200</v>
+      </c>
+      <c r="O5" s="4">
+        <v>42903</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="B6" s="1">
+        <v>777777777</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1">
+        <v>555</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="1">
         <v>1432523294</v>
       </c>
-      <c r="K5" s="5">
+      <c r="N6" s="5">
         <v>200</v>
       </c>
-      <c r="L5" s="4">
-        <v>42903</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1">
-        <v>555</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1432523294</v>
-      </c>
-      <c r="K6" s="5">
-        <v>200</v>
-      </c>
-      <c r="L6" s="4">
+      <c r="O6" s="4">
         <v>42904</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Importação completa, criação da primeira view
</commit_message>
<xml_diff>
--- a/public/sample_titulos.xlsx
+++ b/public/sample_titulos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>NOME</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>BAURU</t>
+  </si>
+  <si>
+    <t>PEDERNEIRAS</t>
   </si>
 </sst>
 </file>
@@ -192,6 +195,39 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -228,6 +264,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -243,42 +282,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -358,20 +361,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:O6" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15">
   <tableColumns count="15">
     <tableColumn id="1" name="NOME" dataDxfId="14"/>
-    <tableColumn id="13" name="RG" dataDxfId="2"/>
-    <tableColumn id="2" name="ESCOLA" dataDxfId="13"/>
-    <tableColumn id="15" name="ESTADO" dataDxfId="0"/>
-    <tableColumn id="14" name="CIDADE" dataDxfId="1"/>
-    <tableColumn id="3" name="TURMA" dataDxfId="12"/>
-    <tableColumn id="4" name="PERIODO" dataDxfId="11"/>
-    <tableColumn id="5" name="TITULO" dataDxfId="10"/>
-    <tableColumn id="6" name="RESPONSAVEL" dataDxfId="9"/>
-    <tableColumn id="7" name="CELULAR" dataDxfId="8"/>
-    <tableColumn id="8" name="TELEFONE" dataDxfId="7"/>
-    <tableColumn id="9" name="TELEFONE2" dataDxfId="6"/>
-    <tableColumn id="10" name="CELULAR2" dataDxfId="5"/>
-    <tableColumn id="11" name="VALOR" dataDxfId="4"/>
-    <tableColumn id="12" name="VENCIMENTO" dataDxfId="3"/>
+    <tableColumn id="13" name="RG" dataDxfId="13"/>
+    <tableColumn id="2" name="ESCOLA" dataDxfId="12"/>
+    <tableColumn id="15" name="ESTADO" dataDxfId="11"/>
+    <tableColumn id="14" name="CIDADE" dataDxfId="10"/>
+    <tableColumn id="3" name="TURMA" dataDxfId="9"/>
+    <tableColumn id="4" name="PERIODO" dataDxfId="8"/>
+    <tableColumn id="5" name="TITULO" dataDxfId="7"/>
+    <tableColumn id="6" name="RESPONSAVEL" dataDxfId="6"/>
+    <tableColumn id="7" name="CELULAR" dataDxfId="5"/>
+    <tableColumn id="8" name="TELEFONE" dataDxfId="4"/>
+    <tableColumn id="9" name="TELEFONE2" dataDxfId="3"/>
+    <tableColumn id="10" name="CELULAR2" dataDxfId="2"/>
+    <tableColumn id="11" name="VALOR" dataDxfId="1"/>
+    <tableColumn id="12" name="VENCIMENTO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Plan1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -676,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -803,7 +806,7 @@
         <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
Envio de SMS funcionando
</commit_message>
<xml_diff>
--- a/public/sample_titulos.xlsx
+++ b/public/sample_titulos.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BB_DENTAL" localSheetId="0">Plan1!$A$1:$O$6</definedName>
+    <definedName name="BB_DENTAL" localSheetId="0">Plan1!$A$1:$P$6</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>NOME</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>PEDERNEIRAS</t>
+  </si>
+  <si>
+    <t>DATA NASCIMENTO</t>
   </si>
 </sst>
 </file>
@@ -193,40 +196,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <font>
         <b val="0"/>
@@ -246,6 +216,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -264,9 +267,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -288,6 +288,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -341,9 +362,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Plan1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="20"/>
-      <tableStyleElement type="firstRowStripe" dxfId="19"/>
-      <tableStyleElement type="secondRowStripe" dxfId="18"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="firstRowStripe" dxfId="20"/>
+      <tableStyleElement type="secondRowStripe" dxfId="19"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -358,23 +379,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:O6" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15">
-  <tableColumns count="15">
-    <tableColumn id="1" name="NOME" dataDxfId="14"/>
-    <tableColumn id="13" name="RG" dataDxfId="13"/>
-    <tableColumn id="2" name="ESCOLA" dataDxfId="12"/>
-    <tableColumn id="15" name="ESTADO" dataDxfId="11"/>
-    <tableColumn id="14" name="CIDADE" dataDxfId="10"/>
-    <tableColumn id="3" name="TURMA" dataDxfId="9"/>
-    <tableColumn id="4" name="PERIODO" dataDxfId="8"/>
-    <tableColumn id="5" name="TITULO" dataDxfId="7"/>
-    <tableColumn id="6" name="RESPONSAVEL" dataDxfId="6"/>
-    <tableColumn id="7" name="CELULAR" dataDxfId="5"/>
-    <tableColumn id="8" name="TELEFONE" dataDxfId="4"/>
-    <tableColumn id="9" name="TELEFONE2" dataDxfId="3"/>
-    <tableColumn id="10" name="CELULAR2" dataDxfId="2"/>
-    <tableColumn id="11" name="VALOR" dataDxfId="1"/>
-    <tableColumn id="12" name="VENCIMENTO" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:P6" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
+  <tableColumns count="16">
+    <tableColumn id="1" name="NOME" dataDxfId="15"/>
+    <tableColumn id="16" name="DATA NASCIMENTO" dataDxfId="0"/>
+    <tableColumn id="13" name="RG" dataDxfId="14"/>
+    <tableColumn id="2" name="ESCOLA" dataDxfId="13"/>
+    <tableColumn id="15" name="ESTADO" dataDxfId="12"/>
+    <tableColumn id="14" name="CIDADE" dataDxfId="11"/>
+    <tableColumn id="3" name="TURMA" dataDxfId="10"/>
+    <tableColumn id="4" name="PERIODO" dataDxfId="9"/>
+    <tableColumn id="5" name="TITULO" dataDxfId="8"/>
+    <tableColumn id="6" name="RESPONSAVEL" dataDxfId="7"/>
+    <tableColumn id="7" name="CELULAR" dataDxfId="6"/>
+    <tableColumn id="8" name="TELEFONE" dataDxfId="5"/>
+    <tableColumn id="9" name="TELEFONE2" dataDxfId="4"/>
+    <tableColumn id="10" name="CELULAR2" dataDxfId="3"/>
+    <tableColumn id="11" name="VALOR" dataDxfId="2"/>
+    <tableColumn id="12" name="VENCIMENTO" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Plan1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,288 +699,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
-    <col min="3" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="12.5703125" style="1"/>
+    <col min="2" max="3" width="22.42578125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="20" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
+        <v>33813</v>
+      </c>
+      <c r="C2" s="1">
         <v>487562847</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>111</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>1432523294</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="5">
+      <c r="O2" s="5">
         <v>100</v>
       </c>
-      <c r="O2" s="4">
+      <c r="P2" s="4">
         <v>42900</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
+        <v>33814</v>
+      </c>
+      <c r="C3" s="1">
         <v>444444444</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>222</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>1432523294</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O3" s="5">
         <v>150</v>
       </c>
-      <c r="O3" s="4">
+      <c r="P3" s="4">
         <v>42901</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
+        <v>33815</v>
+      </c>
+      <c r="C4" s="1">
         <v>555555555</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>333</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1432523294</v>
       </c>
       <c r="L4" s="1">
         <v>1432523294</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="1">
+        <v>1432523294</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>150.56</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <v>42902</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
+        <v>33816</v>
+      </c>
+      <c r="C5" s="1">
         <v>666666666</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>444</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>1432523294</v>
       </c>
-      <c r="N5" s="5">
+      <c r="O5" s="5">
         <v>200</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="4">
         <v>42903</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
+        <v>33817</v>
+      </c>
+      <c r="C6" s="1">
         <v>777777777</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>555</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>1432523294</v>
       </c>
-      <c r="N6" s="5">
+      <c r="O6" s="5">
         <v>200</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <v>42904</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Criação dos repositorios que faltavam
</commit_message>
<xml_diff>
--- a/public/sample_titulos.xlsx
+++ b/public/sample_titulos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>NOME</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>DATA NASCIMENTO</t>
+  </si>
+  <si>
+    <t>14981225509</t>
   </si>
 </sst>
 </file>
@@ -198,6 +201,39 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -216,39 +252,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -267,6 +270,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -282,9 +288,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -382,21 +385,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:P6" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
   <tableColumns count="16">
     <tableColumn id="1" name="NOME" dataDxfId="15"/>
-    <tableColumn id="16" name="DATA NASCIMENTO" dataDxfId="0"/>
-    <tableColumn id="13" name="RG" dataDxfId="14"/>
-    <tableColumn id="2" name="ESCOLA" dataDxfId="13"/>
-    <tableColumn id="15" name="ESTADO" dataDxfId="12"/>
-    <tableColumn id="14" name="CIDADE" dataDxfId="11"/>
-    <tableColumn id="3" name="TURMA" dataDxfId="10"/>
-    <tableColumn id="4" name="PERIODO" dataDxfId="9"/>
-    <tableColumn id="5" name="TITULO" dataDxfId="8"/>
-    <tableColumn id="6" name="RESPONSAVEL" dataDxfId="7"/>
-    <tableColumn id="7" name="CELULAR" dataDxfId="6"/>
-    <tableColumn id="8" name="TELEFONE" dataDxfId="5"/>
-    <tableColumn id="9" name="TELEFONE2" dataDxfId="4"/>
-    <tableColumn id="10" name="CELULAR2" dataDxfId="3"/>
-    <tableColumn id="11" name="VALOR" dataDxfId="2"/>
-    <tableColumn id="12" name="VENCIMENTO" dataDxfId="1"/>
+    <tableColumn id="16" name="DATA NASCIMENTO" dataDxfId="14"/>
+    <tableColumn id="13" name="RG" dataDxfId="13"/>
+    <tableColumn id="2" name="ESCOLA" dataDxfId="12"/>
+    <tableColumn id="15" name="ESTADO" dataDxfId="11"/>
+    <tableColumn id="14" name="CIDADE" dataDxfId="10"/>
+    <tableColumn id="3" name="TURMA" dataDxfId="9"/>
+    <tableColumn id="4" name="PERIODO" dataDxfId="8"/>
+    <tableColumn id="5" name="TITULO" dataDxfId="7"/>
+    <tableColumn id="6" name="RESPONSAVEL" dataDxfId="6"/>
+    <tableColumn id="7" name="CELULAR" dataDxfId="5"/>
+    <tableColumn id="8" name="TELEFONE" dataDxfId="4"/>
+    <tableColumn id="9" name="TELEFONE2" dataDxfId="3"/>
+    <tableColumn id="10" name="CELULAR2" dataDxfId="2"/>
+    <tableColumn id="11" name="VALOR" dataDxfId="1"/>
+    <tableColumn id="12" name="VENCIMENTO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Plan1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -702,7 +705,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,7 +784,7 @@
         <v>33813</v>
       </c>
       <c r="C2" s="1">
-        <v>487562847</v>
+        <v>333333333</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -805,7 +808,7 @@
         <v>15</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L2" s="1">
         <v>1432523294</v>
@@ -852,7 +855,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L3" s="1">
         <v>1432523294</v>
@@ -896,7 +899,7 @@
         <v>23</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L4" s="1">
         <v>1432523294</v>
@@ -946,7 +949,7 @@
         <v>25</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L5" s="1">
         <v>1432523294</v>
@@ -990,7 +993,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L6" s="1">
         <v>1432523294</v>

</xml_diff>